<commit_message>
adding changes from last mtg
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
@@ -440,7 +440,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
@@ -480,7 +480,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -504,7 +504,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="19">
@@ -512,7 +512,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="20">
@@ -560,7 +560,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="26">
@@ -600,7 +600,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="31">
@@ -632,7 +632,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="35">
@@ -640,7 +640,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="36">
@@ -720,7 +720,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="46">
@@ -768,7 +768,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="52">
@@ -824,7 +824,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="59">
@@ -832,7 +832,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="60">
@@ -840,7 +840,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="61">
@@ -872,7 +872,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="65">
@@ -912,7 +912,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="70">
@@ -920,7 +920,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="71">
@@ -984,7 +984,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="79">
@@ -1000,7 +1000,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="81">
@@ -1016,7 +1016,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="83">
@@ -1064,7 +1064,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
@@ -1080,7 +1080,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="91">
@@ -1112,7 +1112,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="95">
@@ -1120,7 +1120,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="96">
@@ -1136,7 +1136,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="98">
@@ -1144,7 +1144,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="99">
@@ -1168,7 +1168,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding alpha to lda(), adding alphas.xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -376,7 +376,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -400,7 +400,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -416,7 +416,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -424,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -432,7 +432,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -440,7 +440,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -448,7 +448,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
@@ -464,7 +464,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="14">
@@ -472,7 +472,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="15">
@@ -480,7 +480,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="16">
@@ -488,7 +488,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
@@ -504,7 +504,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
@@ -520,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
@@ -536,7 +536,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
@@ -568,7 +568,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="27">
@@ -576,7 +576,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="28">
@@ -584,7 +584,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
@@ -592,7 +592,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
@@ -600,7 +600,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="31">
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="32">
@@ -616,7 +616,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="33">
@@ -624,7 +624,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="34">
@@ -632,7 +632,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
@@ -664,7 +664,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="39">
@@ -672,7 +672,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="40">
@@ -680,7 +680,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="41">
@@ -688,7 +688,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="42">
@@ -696,7 +696,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="43">
@@ -712,7 +712,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="45">
@@ -720,7 +720,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="46">
@@ -728,7 +728,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="47">
@@ -736,7 +736,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="48">
@@ -744,7 +744,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="49">
@@ -752,7 +752,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="50">
@@ -776,7 +776,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="53">
@@ -784,7 +784,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="54">
@@ -800,7 +800,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="56">
@@ -808,7 +808,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="57">
@@ -824,7 +824,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="59">
@@ -840,7 +840,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="61">
@@ -848,7 +848,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="62">
@@ -864,7 +864,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="64">
@@ -872,7 +872,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="65">
@@ -880,7 +880,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="66">
@@ -912,7 +912,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="70">
@@ -920,7 +920,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="71">
@@ -928,7 +928,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="72">
@@ -936,7 +936,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="73">
@@ -952,7 +952,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="75">
@@ -960,7 +960,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="76">
@@ -976,7 +976,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="78">
@@ -984,7 +984,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="79">
@@ -1000,7 +1000,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="81">
@@ -1008,7 +1008,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="82">
@@ -1024,7 +1024,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="84">
@@ -1032,7 +1032,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="85">
@@ -1056,7 +1056,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="88">
@@ -1064,7 +1064,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="89">
@@ -1072,7 +1072,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="90">
@@ -1120,7 +1120,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="96">
@@ -1128,7 +1128,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="97">
@@ -1136,7 +1136,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="98">
@@ -1144,7 +1144,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="99">
@@ -1152,7 +1152,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="100">
@@ -1160,7 +1160,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="101">
@@ -1168,7 +1168,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding dummy data files and ldatest.R, which tests posterior probability function
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -376,7 +376,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
@@ -400,7 +400,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
@@ -416,7 +416,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
@@ -424,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
@@ -432,7 +432,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
@@ -440,7 +440,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
@@ -448,7 +448,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="12">
@@ -456,7 +456,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -464,7 +464,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="14">
@@ -472,7 +472,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="15">
@@ -480,7 +480,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -488,7 +488,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
@@ -504,7 +504,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="19">
@@ -520,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
@@ -536,7 +536,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="23">
@@ -544,7 +544,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="24">
@@ -552,7 +552,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="25">
@@ -568,7 +568,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="27">
@@ -576,7 +576,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="28">
@@ -584,7 +584,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="29">
@@ -592,7 +592,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="30">
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="32">
@@ -616,7 +616,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="33">
@@ -624,7 +624,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="34">
@@ -632,7 +632,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="35">
@@ -648,7 +648,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
@@ -656,7 +656,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="38">
@@ -664,7 +664,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
@@ -672,7 +672,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="40">
@@ -680,7 +680,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="41">
@@ -688,7 +688,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="42">
@@ -696,7 +696,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="43">
@@ -712,7 +712,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="45">
@@ -720,7 +720,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="46">
@@ -728,7 +728,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="47">
@@ -736,7 +736,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="48">
@@ -744,7 +744,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
@@ -752,7 +752,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
@@ -760,7 +760,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
@@ -768,7 +768,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="52">
@@ -776,7 +776,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="53">
@@ -784,7 +784,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="54">
@@ -792,7 +792,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="55">
@@ -800,7 +800,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="56">
@@ -808,7 +808,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="57">
@@ -840,7 +840,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="61">
@@ -848,7 +848,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="62">
@@ -864,7 +864,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="64">
@@ -880,7 +880,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="66">
@@ -888,7 +888,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="67">
@@ -912,7 +912,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="70">
@@ -920,7 +920,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="71">
@@ -928,7 +928,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="72">
@@ -936,7 +936,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="73">
@@ -944,7 +944,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="74">
@@ -952,7 +952,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="75">
@@ -960,7 +960,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="76">
@@ -976,7 +976,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="78">
@@ -984,7 +984,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="79">
@@ -1000,7 +1000,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="81">
@@ -1008,7 +1008,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="82">
@@ -1024,7 +1024,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="84">
@@ -1032,7 +1032,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="85">
@@ -1064,7 +1064,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
@@ -1072,7 +1072,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="90">
@@ -1088,7 +1088,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="92">
@@ -1096,7 +1096,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="93">
@@ -1120,7 +1120,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="96">
@@ -1128,7 +1128,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="97">
@@ -1136,7 +1136,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="98">
@@ -1144,7 +1144,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="99">
@@ -1152,7 +1152,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="100">
@@ -1160,7 +1160,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="101">
@@ -1168,7 +1168,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge jdm file into lda.R for testing
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>x</t>
   </si>
@@ -285,36 +285,6 @@
   </si>
   <si>
     <t>90</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>100</t>
   </si>
 </sst>
 </file>
@@ -376,7 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="3">
@@ -384,7 +354,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -392,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -408,7 +378,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -416,7 +386,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
@@ -424,7 +394,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -432,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -440,7 +410,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
@@ -448,7 +418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
@@ -456,7 +426,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="13">
@@ -464,7 +434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
@@ -472,7 +442,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15">
@@ -480,7 +450,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="16">
@@ -488,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="17">
@@ -496,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -504,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -512,7 +482,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
@@ -536,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">
@@ -568,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="27">
@@ -576,7 +546,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -584,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="29">
@@ -592,7 +562,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
@@ -608,7 +578,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="32">
@@ -616,7 +586,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
@@ -624,7 +594,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="34">
@@ -632,7 +602,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
@@ -640,7 +610,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="36">
@@ -648,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="37">
@@ -656,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
@@ -672,7 +642,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="40">
@@ -680,7 +650,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="41">
@@ -696,7 +666,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="43">
@@ -704,7 +674,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="44">
@@ -720,7 +690,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="46">
@@ -728,7 +698,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="47">
@@ -736,7 +706,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="48">
@@ -744,7 +714,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="49">
@@ -752,7 +722,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="50">
@@ -760,7 +730,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="51">
@@ -776,7 +746,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="53">
@@ -792,7 +762,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="55">
@@ -800,7 +770,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="56">
@@ -808,7 +778,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="57">
@@ -816,7 +786,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="58">
@@ -824,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="59">
@@ -832,7 +802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="60">
@@ -848,7 +818,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="62">
@@ -856,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="63">
@@ -864,7 +834,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="64">
@@ -872,7 +842,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="65">
@@ -880,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
@@ -888,7 +858,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="67">
@@ -896,7 +866,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="68">
@@ -912,7 +882,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="70">
@@ -928,7 +898,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="72">
@@ -936,7 +906,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="73">
@@ -944,7 +914,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="74">
@@ -952,7 +922,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="75">
@@ -968,7 +938,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="77">
@@ -976,7 +946,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="78">
@@ -984,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="79">
@@ -992,7 +962,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="80">
@@ -1008,7 +978,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="82">
@@ -1016,7 +986,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="83">
@@ -1032,7 +1002,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="85">
@@ -1040,7 +1010,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="86">
@@ -1048,7 +1018,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="87">
@@ -1056,7 +1026,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="88">
@@ -1064,7 +1034,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="89">
@@ -1072,7 +1042,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="90">
@@ -1080,7 +1050,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="91">
@@ -1088,86 +1058,6 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
-        <v>91</v>
-      </c>
-      <c r="B92" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
-        <v>92</v>
-      </c>
-      <c r="B93" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
-        <v>93</v>
-      </c>
-      <c r="B94" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
-        <v>95</v>
-      </c>
-      <c r="B96" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
-        <v>96</v>
-      </c>
-      <c r="B97" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
-        <v>97</v>
-      </c>
-      <c r="B98" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
-        <v>98</v>
-      </c>
-      <c r="B99" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>99</v>
-      </c>
-      <c r="B100" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
-        <v>100</v>
-      </c>
-      <c r="B101" t="n">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding loop for multiple runs of mutual information
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -346,7 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -362,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5">
@@ -378,7 +378,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
@@ -386,7 +386,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
@@ -394,7 +394,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -402,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="10">
@@ -410,7 +410,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="11">
@@ -418,7 +418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -434,7 +434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="14">
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15">
@@ -450,7 +450,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -458,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="17">
@@ -466,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -474,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="19">
@@ -482,7 +482,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
@@ -490,7 +490,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="21">
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="22">
@@ -506,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">
@@ -514,7 +514,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
@@ -522,7 +522,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
@@ -538,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="27">
@@ -546,7 +546,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="28">
@@ -554,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="29">
@@ -562,7 +562,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="30">
@@ -570,7 +570,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="31">
@@ -578,7 +578,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="32">
@@ -586,7 +586,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="33">
@@ -594,7 +594,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="34">
@@ -602,7 +602,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="35">
@@ -618,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="37">
@@ -626,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="38">
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
@@ -642,7 +642,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="40">
@@ -650,7 +650,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="41">
@@ -658,7 +658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="42">
@@ -666,7 +666,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="43">
@@ -674,7 +674,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="44">
@@ -698,7 +698,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="47">
@@ -706,7 +706,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
@@ -714,7 +714,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="49">
@@ -722,7 +722,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
@@ -730,7 +730,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
@@ -738,7 +738,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="52">
@@ -746,7 +746,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="53">
@@ -754,7 +754,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
@@ -762,7 +762,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="55">
@@ -770,7 +770,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
@@ -778,7 +778,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="57">
@@ -794,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="59">
@@ -802,7 +802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="60">
@@ -810,7 +810,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="61">
@@ -818,7 +818,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="62">
@@ -826,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="63">
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
@@ -858,7 +858,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="67">
@@ -874,7 +874,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="69">
@@ -890,7 +890,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="71">
@@ -898,7 +898,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="72">
@@ -906,7 +906,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="73">
@@ -914,7 +914,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="74">
@@ -930,7 +930,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="76">
@@ -938,7 +938,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="77">
@@ -946,7 +946,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="78">
@@ -954,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="79">
@@ -970,7 +970,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="81">
@@ -978,7 +978,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="82">
@@ -986,7 +986,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="83">
@@ -994,7 +994,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="84">
@@ -1002,7 +1002,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="85">
@@ -1010,7 +1010,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="86">
@@ -1018,7 +1018,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="87">
@@ -1026,7 +1026,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="88">
@@ -1034,7 +1034,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
@@ -1042,7 +1042,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="90">
@@ -1050,7 +1050,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="91">
@@ -1058,7 +1058,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting mutual info per document
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -346,7 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
@@ -362,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -370,7 +370,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
@@ -394,7 +394,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9">
@@ -402,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -418,7 +418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
@@ -434,7 +434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="14">
@@ -450,7 +450,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -458,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
@@ -466,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -474,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="19">
@@ -490,7 +490,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="22">
@@ -506,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="23">
@@ -514,7 +514,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="24">
@@ -522,7 +522,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="25">
@@ -530,7 +530,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="26">
@@ -538,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="27">
@@ -546,7 +546,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -554,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
@@ -562,7 +562,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="30">
@@ -570,7 +570,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="31">
@@ -578,7 +578,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="32">
@@ -586,7 +586,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="33">
@@ -594,7 +594,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="34">
@@ -602,7 +602,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="35">
@@ -610,7 +610,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="36">
@@ -618,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="37">
@@ -626,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="38">
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="39">
@@ -642,7 +642,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="40">
@@ -650,7 +650,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="41">
@@ -666,7 +666,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="43">
@@ -674,7 +674,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="44">
@@ -682,7 +682,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="45">
@@ -690,7 +690,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
@@ -714,7 +714,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="49">
@@ -730,7 +730,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="51">
@@ -738,7 +738,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="52">
@@ -746,7 +746,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="53">
@@ -762,7 +762,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="55">
@@ -770,7 +770,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="56">
@@ -778,7 +778,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="57">
@@ -786,7 +786,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="58">
@@ -794,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="59">
@@ -802,7 +802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="60">
@@ -810,7 +810,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="61">
@@ -818,7 +818,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="62">
@@ -826,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="63">
@@ -834,7 +834,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="64">
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
@@ -858,7 +858,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="67">
@@ -882,7 +882,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="70">
@@ -906,7 +906,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="73">
@@ -922,7 +922,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="75">
@@ -930,7 +930,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="76">
@@ -946,7 +946,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="78">
@@ -954,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="79">
@@ -962,7 +962,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="80">
@@ -970,7 +970,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="81">
@@ -978,7 +978,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="82">
@@ -986,7 +986,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="83">
@@ -994,7 +994,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="84">
@@ -1002,7 +1002,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="85">
@@ -1010,7 +1010,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="86">
@@ -1018,7 +1018,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="87">
@@ -1026,7 +1026,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="88">
@@ -1034,7 +1034,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="89">
@@ -1042,7 +1042,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="90">
@@ -1050,7 +1050,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="91">
@@ -1058,7 +1058,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run with 10000 mutual information values
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -346,7 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
@@ -354,7 +354,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
@@ -362,7 +362,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -370,7 +370,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -378,7 +378,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
@@ -386,7 +386,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
@@ -394,7 +394,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
@@ -402,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="10">
@@ -410,7 +410,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
@@ -418,7 +418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
@@ -426,7 +426,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
@@ -434,7 +434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="14">
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
@@ -458,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
@@ -466,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="18">
@@ -474,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="19">
@@ -482,7 +482,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="20">
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="22">
@@ -506,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">
@@ -514,7 +514,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
@@ -530,7 +530,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="26">
@@ -538,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="27">
@@ -546,7 +546,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="28">
@@ -554,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="29">
@@ -562,7 +562,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
@@ -570,7 +570,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="31">
@@ -578,7 +578,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="32">
@@ -586,7 +586,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="33">
@@ -594,7 +594,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="34">
@@ -602,7 +602,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="35">
@@ -610,7 +610,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="36">
@@ -618,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="37">
@@ -626,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
@@ -634,7 +634,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="39">
@@ -658,7 +658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="42">
@@ -666,7 +666,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="43">
@@ -674,7 +674,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="44">
@@ -682,7 +682,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="45">
@@ -698,7 +698,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="47">
@@ -706,7 +706,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="48">
@@ -714,7 +714,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="49">
@@ -722,7 +722,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="50">
@@ -738,7 +738,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="52">
@@ -754,7 +754,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="54">
@@ -762,7 +762,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="55">
@@ -770,7 +770,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="56">
@@ -778,7 +778,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="57">
@@ -794,7 +794,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="59">
@@ -802,7 +802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="60">
@@ -818,7 +818,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="62">
@@ -826,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="63">
@@ -834,7 +834,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="64">
@@ -842,7 +842,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="65">
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
@@ -858,7 +858,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="67">
@@ -866,7 +866,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="68">
@@ -874,7 +874,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="69">
@@ -882,7 +882,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="70">
@@ -890,7 +890,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="71">
@@ -898,7 +898,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="72">
@@ -922,7 +922,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="75">
@@ -930,7 +930,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="76">
@@ -938,7 +938,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="77">
@@ -946,7 +946,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="78">
@@ -954,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="79">
@@ -962,7 +962,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="80">
@@ -970,7 +970,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="81">
@@ -986,7 +986,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="83">
@@ -994,7 +994,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="84">
@@ -1002,7 +1002,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="85">
@@ -1018,7 +1018,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="87">
@@ -1026,7 +1026,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="88">
@@ -1034,7 +1034,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
@@ -1042,7 +1042,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="90">
@@ -1050,7 +1050,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="91">

</xml_diff>

<commit_message>
adding post processing step
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -346,7 +346,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -370,7 +370,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
@@ -378,7 +378,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -386,7 +386,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="8">
@@ -394,7 +394,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
@@ -402,7 +402,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -410,7 +410,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="11">
@@ -418,7 +418,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="12">
@@ -426,7 +426,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
@@ -434,7 +434,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="14">
@@ -442,7 +442,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="15">
@@ -450,7 +450,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -458,7 +458,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="17">
@@ -466,7 +466,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="18">
@@ -474,7 +474,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="19">
@@ -490,7 +490,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="22">
@@ -506,7 +506,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23">
@@ -514,7 +514,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="24">
@@ -522,7 +522,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="25">
@@ -530,7 +530,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="26">
@@ -538,7 +538,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="27">
@@ -546,7 +546,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
@@ -554,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="29">
@@ -562,7 +562,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="30">
@@ -586,7 +586,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="33">
@@ -602,7 +602,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="35">
@@ -618,7 +618,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="37">
@@ -626,7 +626,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="38">
@@ -642,7 +642,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="40">
@@ -658,7 +658,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="42">
@@ -674,7 +674,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="44">
@@ -690,7 +690,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="46">
@@ -706,7 +706,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
@@ -714,7 +714,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="49">
@@ -722,7 +722,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="50">
@@ -730,7 +730,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="51">
@@ -738,7 +738,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="52">
@@ -754,7 +754,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="54">
@@ -762,7 +762,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="55">
@@ -786,7 +786,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="58">
@@ -802,7 +802,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="60">
@@ -810,7 +810,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="61">
@@ -818,7 +818,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="62">
@@ -826,7 +826,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="63">
@@ -834,7 +834,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="64">
@@ -850,7 +850,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
@@ -858,7 +858,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="67">
@@ -866,7 +866,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="68">
@@ -874,7 +874,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="69">
@@ -882,7 +882,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="70">
@@ -890,7 +890,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="71">
@@ -898,7 +898,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="72">
@@ -906,7 +906,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="73">
@@ -914,7 +914,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="74">
@@ -930,7 +930,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="76">
@@ -946,7 +946,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="78">
@@ -954,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="79">
@@ -962,7 +962,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="80">
@@ -970,7 +970,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="81">
@@ -986,7 +986,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="83">
@@ -994,7 +994,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="84">
@@ -1002,7 +1002,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="85">
@@ -1010,7 +1010,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="86">
@@ -1026,7 +1026,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="88">
@@ -1042,7 +1042,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="90">
@@ -1050,7 +1050,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="91">
@@ -1058,7 +1058,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding median lists for postProcessing.R
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>x</t>
   </si>
@@ -165,6 +165,81 @@
   </si>
   <si>
     <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
   </si>
 </sst>
 </file>
@@ -226,7 +301,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
@@ -234,7 +309,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -242,7 +317,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -258,7 +333,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -266,7 +341,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
@@ -274,7 +349,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
@@ -282,7 +357,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
@@ -290,7 +365,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
@@ -306,7 +381,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
@@ -322,7 +397,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="15">
@@ -330,7 +405,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="16">
@@ -338,7 +413,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="17">
@@ -346,7 +421,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="18">
@@ -354,7 +429,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="19">
@@ -362,7 +437,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="20">
@@ -370,7 +445,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="21">
@@ -378,7 +453,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="22">
@@ -386,7 +461,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23">
@@ -394,7 +469,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="24">
@@ -402,7 +477,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="25">
@@ -410,7 +485,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="26">
@@ -426,7 +501,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="28">
@@ -434,7 +509,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
@@ -466,7 +541,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
@@ -474,7 +549,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="34">
@@ -482,7 +557,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="35">
@@ -490,7 +565,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="36">
@@ -498,7 +573,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="37">
@@ -530,7 +605,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="41">
@@ -538,7 +613,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="42">
@@ -554,7 +629,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="44">
@@ -562,7 +637,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="45">
@@ -570,7 +645,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="46">
@@ -578,7 +653,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="47">
@@ -586,7 +661,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="48">
@@ -594,7 +669,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
@@ -602,7 +677,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="50">
@@ -618,6 +693,206 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="n">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding partial labeling file
</commit_message>
<xml_diff>
--- a/ldaresults_curatedafg_100_5.xlsx
+++ b/ldaresults_curatedafg_100_5.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>x</t>
   </si>
@@ -165,81 +165,6 @@
   </si>
   <si>
     <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>75</t>
   </si>
 </sst>
 </file>
@@ -301,7 +226,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -309,7 +234,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
@@ -317,7 +242,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
@@ -325,7 +250,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="6">
@@ -333,7 +258,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -341,7 +266,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -357,7 +282,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
@@ -365,7 +290,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="11">
@@ -373,7 +298,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="12">
@@ -381,7 +306,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="13">
@@ -389,7 +314,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="14">
@@ -397,7 +322,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="15">
@@ -405,7 +330,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="16">
@@ -413,7 +338,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
@@ -421,7 +346,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="18">
@@ -429,7 +354,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="19">
@@ -437,7 +362,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="20">
@@ -445,7 +370,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21">
@@ -453,7 +378,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="22">
@@ -461,7 +386,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="23">
@@ -469,7 +394,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
@@ -477,7 +402,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="25">
@@ -485,7 +410,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="26">
@@ -501,7 +426,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="28">
@@ -509,7 +434,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="29">
@@ -517,7 +442,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="30">
@@ -525,7 +450,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="31">
@@ -541,7 +466,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="33">
@@ -549,7 +474,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="34">
@@ -565,7 +490,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="36">
@@ -573,7 +498,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="37">
@@ -581,7 +506,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="38">
@@ -589,7 +514,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="39">
@@ -597,7 +522,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="40">
@@ -605,7 +530,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="41">
@@ -629,7 +554,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="44">
@@ -637,7 +562,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="45">
@@ -645,7 +570,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="46">
@@ -661,7 +586,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="48">
@@ -669,7 +594,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="49">
@@ -693,207 +618,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" t="n">
         <v>3.0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>67</v>
-      </c>
-      <c r="B68" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
-        <v>71</v>
-      </c>
-      <c r="B72" t="n">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-      <c r="B73" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
-        <v>73</v>
-      </c>
-      <c r="B74" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
-        <v>74</v>
-      </c>
-      <c r="B75" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" t="n">
-        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>